<commit_message>
PerkinElmer Winlab32 and Nexion350x fixes
- Because we match keywords with ".startswith", there is a possibility for having ARs where multiple analyses match a single row.  This causes a warning and ignores the row.
- Keywords are not lowercased in their conversion from the values in the input document.
</commit_message>
<xml_diff>
--- a/src/senaite/instruments/tests/files/instruments/bruker/s8tiger/DU-0001-234987347.xlsx
+++ b/src/senaite/instruments/tests/files/instruments/bruker/s8tiger/DU-0001-234987347.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Folha1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Concentrations" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Folha2" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Folha3" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
@@ -340,10 +340,10 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="G44" activeCellId="0" sqref="G44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.7"/>
@@ -774,10 +774,10 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B3 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -797,10 +797,10 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B3 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>